<commit_message>
homeword excel sheet has been modified
</commit_message>
<xml_diff>
--- a/hw2.xlsx
+++ b/hw2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faysal/Desktop/My Computer/D/TA/Assignment-2/Dataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faysal/Desktop/My Computer/D/TA/2018/Assignment-2/Dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="1120" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="-33360" yWindow="-7540" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="13">
   <si>
     <t>Channel #1</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Channel #5</t>
   </si>
   <si>
-    <t>potential vulnerablity (Leaking sensitive information/Violates user privacy/Causes security threat)</t>
-  </si>
-  <si>
     <t>Chain#</t>
   </si>
   <si>
@@ -54,6 +51,21 @@
   </si>
   <si>
     <t>Manual / Automatic</t>
+  </si>
+  <si>
+    <t>potential vulnerablity (Violates user privacy/Causes security threat)</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>Automatic</t>
+  </si>
+  <si>
+    <t>Violates User Privacy</t>
+  </si>
+  <si>
+    <t>Cause Security Threat</t>
   </si>
 </sst>
 </file>
@@ -371,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -382,204 +394,494 @@
     <col min="2" max="3" width="53.1640625" customWidth="1"/>
     <col min="5" max="5" width="28.1640625" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" customWidth="1"/>
-    <col min="8" max="8" width="15.5" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="20.5" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
     <col min="10" max="10" width="17.33203125" customWidth="1"/>
-    <col min="11" max="11" width="15.5" customWidth="1"/>
+    <col min="11" max="11" width="18.83203125" customWidth="1"/>
     <col min="12" max="12" width="15.1640625" customWidth="1"/>
-    <col min="13" max="13" width="14.5" customWidth="1"/>
+    <col min="13" max="13" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
       </c>
       <c r="K1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L1" t="s">
         <v>4</v>
       </c>
       <c r="M1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>